<commit_message>
feat: add some colors
</commit_message>
<xml_diff>
--- a/Downloads Organizer Config.xlsx
+++ b/Downloads Organizer Config.xlsx
@@ -125,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ConfigTable" displayName="ConfigTable" ref="A1:B33" headerRowCount="1">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ConfigTable" displayName="ConfigTable" ref="A1:B34" headerRowCount="1">
+  <autoFilter ref="A1:B34"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Folder Name"/>
     <tableColumn id="2" name="Extension"/>
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,36 +711,36 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Videos</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>mp3</t>
+          <t>gif</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LaTex</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>tex</t>
+          <t>mp3</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Executable</t>
+          <t>LaTex</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>exe</t>
+          <t>tex</t>
         </is>
       </c>
     </row>
@@ -752,19 +752,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>msi</t>
+          <t>exe</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Programming</t>
+          <t>Executable</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>py</t>
+          <t>msi</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>json</t>
+          <t>py</t>
         </is>
       </c>
     </row>
@@ -788,7 +788,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>db</t>
+          <t>json</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>yml</t>
+          <t>db</t>
         </is>
       </c>
     </row>
@@ -812,17 +812,29 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>yaml</t>
+          <t>yml</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>Programming</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>yaml</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>Outlook</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>msg</t>
         </is>

</xml_diff>